<commit_message>
Corrige status de arco tiete
</commit_message>
<xml_diff>
--- a/input/monitoramento.xlsx
+++ b/input/monitoramento.xlsx
@@ -1942,10 +1942,10 @@
   <dimension ref="A1:CE22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BR2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="BS2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BS28" sqref="BS28"/>
+      <selection pane="bottomRight" activeCell="CD4" sqref="CD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15"/>
@@ -3027,7 +3027,7 @@
         <v>95</v>
       </c>
       <c r="CD4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="CE4" s="5" t="s">
         <v>152</v>

</xml_diff>